<commit_message>
Tai full project advance testing len lan dau
</commit_message>
<xml_diff>
--- a/login-results.xlsx
+++ b/login-results.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>Username</t>
   </si>
@@ -35,16 +35,13 @@
     <t>PASS</t>
   </si>
   <si>
-    <t>2025-04-09 15:04:35</t>
+    <t>2025-04-14 13:05:52</t>
   </si>
   <si>
     <t>locked_out_user</t>
   </si>
   <si>
     <t>FAIL</t>
-  </si>
-  <si>
-    <t>2025-04-09 15:04:36</t>
   </si>
   <si>
     <t>invalid_user</t>
@@ -146,21 +143,21 @@
         <v>9</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s" s="0">
         <v>9</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>